<commit_message>
Include dependencies on pack
</commit_message>
<xml_diff>
--- a/Itamaram.Excel.SpecFlowPlugin.IntegrationTests/Features/Book1.xlsx
+++ b/Itamaram.Excel.SpecFlowPlugin.IntegrationTests/Features/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\SpecFlow.Plugin.Base\Itamaram.Excel.SpecFlowPlugin.IntegrationTests\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB148277-C273-419A-A2AC-0A20E9162BE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05583349-21FF-4778-907B-CFB82F8C8AE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{48E912E3-F508-4588-AE82-830AA8426E11}"/>
   </bookViews>
@@ -380,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645C1B7A-D566-422F-AC14-AD15B2F1B8C4}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -399,17 +399,6 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>